<commit_message>
membuat halaman data siswa dan juga fitur tambah data siswa
</commit_message>
<xml_diff>
--- a/assets/example-file/file-example.xlsx
+++ b/assets/example-file/file-example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\webcrafters\project\team-project\kita-bersuara-project\assets\example-file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8CD36D-9A53-477F-A08D-02C925F98F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD683B1-4D54-4E76-B016-EEFB9F1AF2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47FA2747-1A0A-42AD-B5B9-B422654C68C5}"/>
   </bookViews>
@@ -102,9 +102,6 @@
     <t>Muhammad Nurwakhid M.</t>
   </si>
   <si>
-    <t>Muhammad Zaidan Yaafi'</t>
-  </si>
-  <si>
     <t>Mutiara</t>
   </si>
   <si>
@@ -156,12 +153,6 @@
     <t>0000000001</t>
   </si>
   <si>
-    <t>0000000002</t>
-  </si>
-  <si>
-    <t>0000000003</t>
-  </si>
-  <si>
     <t>0000000004</t>
   </si>
   <si>
@@ -268,6 +259,15 @@
   </si>
   <si>
     <t>0000000039</t>
+  </si>
+  <si>
+    <t>00000000042</t>
+  </si>
+  <si>
+    <t>00000000043</t>
+  </si>
+  <si>
+    <t>Muhammad Zaidan Yaafi</t>
   </si>
 </sst>
 </file>
@@ -632,11 +632,12 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" customWidth="1"/>
   </cols>
@@ -653,432 +654,432 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>42</v>
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2">
+        <v>12345678</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>43</v>
+      <c r="A3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="2">
+        <v>12345678</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>44</v>
+      <c r="A4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="2">
+        <v>12345678</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>45</v>
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="2">
+        <v>12345678</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>46</v>
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="2">
+        <v>12345678</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>47</v>
+      <c r="A7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="2">
+        <v>12345678</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>48</v>
+      <c r="A8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2">
+        <v>12345678</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>49</v>
+      <c r="A9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="2">
+        <v>12345678</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>50</v>
+      <c r="A10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="2">
+        <v>12345678</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>51</v>
+      <c r="A11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="2">
+        <v>12345678</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>52</v>
+      <c r="A12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="2">
+        <v>12345678</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>53</v>
+      <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12345678</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>54</v>
+      <c r="A14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="2">
+        <v>12345678</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>55</v>
+      <c r="A15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="2">
+        <v>12345678</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>56</v>
+      <c r="A16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="2">
+        <v>12345678</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>57</v>
+      <c r="A17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="2">
+        <v>12345678</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>58</v>
+      <c r="A18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="2">
+        <v>12345678</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>59</v>
+      <c r="A19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="2">
+        <v>12345678</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>60</v>
+      <c r="A20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="2">
+        <v>12345678</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>61</v>
+      <c r="A21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="2">
+        <v>12345678</v>
       </c>
       <c r="C21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="B25" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="B26" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="B27" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="B28" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" s="2" t="s">
+      <c r="B29" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>70</v>
+      <c r="B30" s="2">
+        <v>12345678</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>71</v>
+      <c r="A31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="2">
+        <v>12345678</v>
       </c>
       <c r="C31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" t="s">
-        <v>35</v>
-      </c>
-    </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>73</v>
+      <c r="A33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="2">
+        <v>12345678</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2" t="s">
+      <c r="A34" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>77</v>
+      <c r="B37" s="2">
+        <v>12345678</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>78</v>
+      <c r="A38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="2">
+        <v>12345678</v>
       </c>
       <c r="C38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="C40" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
memperbaiki ui data siswa
</commit_message>
<xml_diff>
--- a/assets/example-file/file-example.xlsx
+++ b/assets/example-file/file-example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\webcrafters\project\team-project\kita-bersuara-project\assets\example-file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kita-bersuara\assets\example-file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD683B1-4D54-4E76-B016-EEFB9F1AF2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03E73E9-7585-4442-9BBC-50823D11F315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47FA2747-1A0A-42AD-B5B9-B422654C68C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{47FA2747-1A0A-42AD-B5B9-B422654C68C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>nisn</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Maheswara Puwa Hadi G.</t>
   </si>
   <si>
-    <t>Mahreta Izza</t>
-  </si>
-  <si>
     <t>Marcello Artasda</t>
   </si>
   <si>
@@ -78,18 +75,9 @@
     <t>Mochamad Risky Subagyo</t>
   </si>
   <si>
-    <t>Ganendra</t>
-  </si>
-  <si>
     <t>Moh. Vicko Nur Ardian</t>
   </si>
   <si>
-    <t>M. Fahrul F.</t>
-  </si>
-  <si>
-    <t>Khalilando</t>
-  </si>
-  <si>
     <t>Muhammad Adji Saputra</t>
   </si>
   <si>
@@ -102,54 +90,21 @@
     <t>Muhammad Nurwakhid M.</t>
   </si>
   <si>
-    <t>Mutiara</t>
-  </si>
-  <si>
-    <t>Nadindra</t>
-  </si>
-  <si>
-    <t>Naufal Haziq</t>
-  </si>
-  <si>
-    <t>Naziratul</t>
-  </si>
-  <si>
     <t>Omega Widyatmaja</t>
   </si>
   <si>
     <t>Pingkan Ferdina Sayidah</t>
   </si>
   <si>
-    <t>Risky Fadhila</t>
-  </si>
-  <si>
-    <t>Rasyadhan</t>
-  </si>
-  <si>
-    <t>Reyvan Farrel A.</t>
-  </si>
-  <si>
     <t>Roval Hidayat</t>
   </si>
   <si>
-    <t>Senja R.S.</t>
-  </si>
-  <si>
-    <t>Virginia Aura</t>
-  </si>
-  <si>
     <t>Winda Setiani</t>
   </si>
   <si>
     <t>Zahra Adientya Putri</t>
   </si>
   <si>
-    <t>Zidane Al Katar</t>
-  </si>
-  <si>
-    <t>Zidane Maulana A.</t>
-  </si>
-  <si>
     <t>0000000001</t>
   </si>
   <si>
@@ -261,20 +216,182 @@
     <t>0000000039</t>
   </si>
   <si>
-    <t>00000000042</t>
-  </si>
-  <si>
-    <t>00000000043</t>
-  </si>
-  <si>
     <t>Muhammad Zaidan Yaafi</t>
+  </si>
+  <si>
+    <t>0000000002</t>
+  </si>
+  <si>
+    <t>0000000003</t>
+  </si>
+  <si>
+    <t>Zidane Maulana Aditya</t>
+  </si>
+  <si>
+    <t>Zidane Arfa Al Katar</t>
+  </si>
+  <si>
+    <t>Virginia Aura Ramadhani</t>
+  </si>
+  <si>
+    <t>Senja Rahmadhiani Septianti</t>
+  </si>
+  <si>
+    <t>Reyvan Andycka Farrel A.</t>
+  </si>
+  <si>
+    <t>Rasyadhan Afdhal Fahza F.</t>
+  </si>
+  <si>
+    <t>Mahreta Izzatul Khusna</t>
+  </si>
+  <si>
+    <t>Moh Ganendra Aditya F.</t>
+  </si>
+  <si>
+    <t>Mohammad Fahrul Alif F.</t>
+  </si>
+  <si>
+    <t>Muhamad Khalilando S.</t>
+  </si>
+  <si>
+    <t>Mutiara Chyntia Dewi</t>
+  </si>
+  <si>
+    <t>Nadindra Pramesti Ken N.</t>
+  </si>
+  <si>
+    <t>Naufal Haziq Bakhtiar</t>
+  </si>
+  <si>
+    <t>Naziratul Wahdhani</t>
+  </si>
+  <si>
+    <t>Ramadhani Risky Fadilah</t>
+  </si>
+  <si>
+    <t>pnz6fw</t>
+  </si>
+  <si>
+    <t>4w6gah</t>
+  </si>
+  <si>
+    <t>b4zuyk</t>
+  </si>
+  <si>
+    <t>vdjcg7</t>
+  </si>
+  <si>
+    <t>492oca</t>
+  </si>
+  <si>
+    <t>3rhyq4</t>
+  </si>
+  <si>
+    <t>5lemmm</t>
+  </si>
+  <si>
+    <t>ydxzgc</t>
+  </si>
+  <si>
+    <t>pt0gm4</t>
+  </si>
+  <si>
+    <t>gqw8g3</t>
+  </si>
+  <si>
+    <t>a4aw45</t>
+  </si>
+  <si>
+    <t>c5j1ko</t>
+  </si>
+  <si>
+    <t>2jmrky</t>
+  </si>
+  <si>
+    <t>kvakbg</t>
+  </si>
+  <si>
+    <t>tt03vj</t>
+  </si>
+  <si>
+    <t>qrvcgx</t>
+  </si>
+  <si>
+    <t>gkpy9s</t>
+  </si>
+  <si>
+    <t>35fnbz</t>
+  </si>
+  <si>
+    <t>jej9ye</t>
+  </si>
+  <si>
+    <t>j8xmkq</t>
+  </si>
+  <si>
+    <t>h2uckw</t>
+  </si>
+  <si>
+    <t>32vivl</t>
+  </si>
+  <si>
+    <t>t6e0sp</t>
+  </si>
+  <si>
+    <t>a92gs1</t>
+  </si>
+  <si>
+    <t>k5l0t0</t>
+  </si>
+  <si>
+    <t>p59570</t>
+  </si>
+  <si>
+    <t>kucq5d</t>
+  </si>
+  <si>
+    <t>7ua5g8</t>
+  </si>
+  <si>
+    <t>mxxybs</t>
+  </si>
+  <si>
+    <t>yl4pe8</t>
+  </si>
+  <si>
+    <t>gdbo86</t>
+  </si>
+  <si>
+    <t>fqr6dz</t>
+  </si>
+  <si>
+    <t>mab6ji</t>
+  </si>
+  <si>
+    <t>dskwr4</t>
+  </si>
+  <si>
+    <t>e5k460</t>
+  </si>
+  <si>
+    <t>pww1iy</t>
+  </si>
+  <si>
+    <t>ho2410</t>
+  </si>
+  <si>
+    <t>ul3jo8</t>
+  </si>
+  <si>
+    <t>0mjz9s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +406,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -311,10 +434,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD7529A-2641-4202-B1CF-C905355650B9}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,10 +781,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="2">
-        <v>12345678</v>
+        <v>26</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -666,10 +792,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="2">
-        <v>12345678</v>
+        <v>64</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -677,10 +803,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="2">
-        <v>12345678</v>
+        <v>65</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -688,10 +814,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="2">
-        <v>12345678</v>
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -699,10 +825,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="2">
-        <v>12345678</v>
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -710,10 +836,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="2">
-        <v>12345678</v>
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -721,131 +847,131 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="2">
-        <v>12345678</v>
+        <v>30</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="2">
-        <v>12345678</v>
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="2">
-        <v>12345678</v>
+        <v>32</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="2">
-        <v>12345678</v>
+        <v>33</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="2">
-        <v>12345678</v>
+        <v>34</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="2">
-        <v>12345678</v>
+        <v>35</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="2">
-        <v>12345678</v>
+        <v>36</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="2">
-        <v>12345678</v>
+        <v>37</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="2">
-        <v>12345678</v>
+        <v>38</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="2">
-        <v>12345678</v>
+        <v>39</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="2">
-        <v>12345678</v>
+        <v>40</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="2">
-        <v>12345678</v>
+        <v>41</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -853,120 +979,120 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="2">
-        <v>12345678</v>
+        <v>42</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="2">
-        <v>12345678</v>
+        <v>43</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="2">
-        <v>12345678</v>
+        <v>44</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="2">
-        <v>12345678</v>
+        <v>45</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="2">
-        <v>12345678</v>
+        <v>46</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="2">
-        <v>12345678</v>
+        <v>47</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="2">
-        <v>12345678</v>
+        <v>48</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="2">
-        <v>12345678</v>
+        <v>49</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="2">
-        <v>12345678</v>
+        <v>50</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="2">
-        <v>12345678</v>
+        <v>51</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="2">
-        <v>12345678</v>
+        <v>52</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -974,32 +1100,32 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="2">
-        <v>12345678</v>
+        <v>53</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="2">
-        <v>12345678</v>
+        <v>54</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="2">
-        <v>12345678</v>
+        <v>55</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -1007,43 +1133,43 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="2">
-        <v>12345678</v>
+        <v>56</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="2">
-        <v>12345678</v>
+        <v>57</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="2">
-        <v>12345678</v>
+        <v>58</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="2">
-        <v>12345678</v>
+        <v>59</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
@@ -1051,35 +1177,35 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" s="2">
-        <v>12345678</v>
+        <v>60</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="2">
-        <v>12345678</v>
+        <v>61</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="2">
-        <v>12345678</v>
+        <v>62</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>